<commit_message>
SLIGHTLY CHANGE AND NEW DATA
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -13,12 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="70 crowdfunding sites" sheetId="4" r:id="rId1"/>
-    <sheet name="Visitor_view" sheetId="5" r:id="rId2"/>
-    <sheet name="General" sheetId="1" r:id="rId3"/>
-    <sheet name="Bridge or Mezz Loan" sheetId="2" r:id="rId4"/>
-    <sheet name="Acquisition" sheetId="3" r:id="rId5"/>
+    <sheet name="Grading criteria" sheetId="7" r:id="rId2"/>
+    <sheet name="Visitor_view" sheetId="5" r:id="rId3"/>
+    <sheet name="General" sheetId="1" r:id="rId4"/>
+    <sheet name="Bridge or Mezz Loan" sheetId="2" r:id="rId5"/>
+    <sheet name="Acquisition" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="501">
   <si>
     <t>Company</t>
   </si>
@@ -390,10 +391,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Loan</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.fastfundingservice.com/real/?gclid=Cj0KCQjw1q3VBRCFARIsAPHJXrHuDbdu9q9WH2uGk3Aw70xb-kgTy-M7YWfcW3kGNVzdbPwNXT6390gaAkugEALw_wcB</t>
   </si>
   <si>
@@ -409,13 +406,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.goodwinlaw.com/services/industries/crowdfunding</t>
-  </si>
-  <si>
-    <t>Goodwin</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>Residential portfolio</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -597,9 +587,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>massventure</t>
-  </si>
-  <si>
     <t>?(not safe, might be fraud)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1139,14 +1126,6 @@
   </si>
   <si>
     <t>DiversyFund</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>category</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -1768,6 +1747,36 @@
   <si>
     <t>Unknown</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.breit.com/</t>
+  </si>
+  <si>
+    <t>Blackstone</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>raise</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>commercial raise</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.therealestatecrowdfundingreview.com/top-14-nonaccredited-realestate</t>
+  </si>
+  <si>
+    <t>massventure</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feature</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2295,6 +2304,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2324,24 +2351,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2629,10 +2638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2646,1042 +2655,1060 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>316</v>
+        <v>499</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>315</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="68" t="s">
-        <v>314</v>
+      <c r="A2" s="58" t="s">
+        <v>310</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="67" t="s">
-        <v>311</v>
+      <c r="A3" s="57" t="s">
+        <v>307</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="65" t="s">
-        <v>307</v>
+      <c r="A4" s="55" t="s">
+        <v>303</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="65" t="s">
-        <v>303</v>
+      <c r="A6" s="55" t="s">
+        <v>299</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="65" t="s">
-        <v>300</v>
+      <c r="A7" s="55" t="s">
+        <v>296</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="65" t="s">
-        <v>298</v>
+      <c r="A8" s="55" t="s">
+        <v>294</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="55" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="56" t="s">
+        <v>289</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="56" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="56" t="s">
+        <v>277</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="57" t="s">
         <v>273</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="65" t="s">
-        <v>296</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="66" t="s">
-        <v>293</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="69" t="s">
-        <v>290</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B15" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="57" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="57" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="58" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="60" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="60" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="66" t="s">
-        <v>287</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="66" t="s">
-        <v>284</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="66" t="s">
-        <v>281</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="67" t="s">
-        <v>277</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="67" t="s">
-        <v>275</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="67" t="s">
-        <v>271</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="67" t="s">
-        <v>267</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="67" t="s">
-        <v>265</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="67" t="s">
-        <v>262</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="67" t="s">
-        <v>260</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B42" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="67" t="s">
-        <v>257</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="68" t="s">
-        <v>255</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="68" t="s">
-        <v>253</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C24" s="7" t="s">
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="68" t="s">
-        <v>250</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="68" t="s">
-        <v>248</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="68" t="s">
-        <v>245</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="68" t="s">
-        <v>243</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="68" t="s">
-        <v>240</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="D43" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="60" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="60" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="60" t="s">
+        <v>498</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="68" t="s">
-        <v>237</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="68" t="s">
-        <v>233</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="70" t="s">
-        <v>227</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="70" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="70" t="s">
-        <v>218</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="70" t="s">
-        <v>215</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="70" t="s">
-        <v>213</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="70" t="s">
-        <v>211</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="70" t="s">
-        <v>208</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C41" s="7" t="s">
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="60" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="70" t="s">
-        <v>201</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="70" t="s">
-        <v>199</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="70" t="s">
-        <v>195</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="70" t="s">
-        <v>191</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="70" t="s">
-        <v>188</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="70" t="s">
-        <v>186</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="70" t="s">
-        <v>184</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="70" t="s">
-        <v>181</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="70" t="s">
-        <v>179</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="70" t="s">
-        <v>173</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="70" t="s">
-        <v>170</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="70" t="s">
-        <v>168</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="70" t="s">
-        <v>163</v>
+      <c r="A56" s="60" t="s">
+        <v>160</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="70" t="s">
-        <v>161</v>
+      <c r="A57" s="60" t="s">
+        <v>158</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="70" t="s">
-        <v>159</v>
+      <c r="A58" s="60" t="s">
+        <v>156</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="70" t="s">
-        <v>154</v>
+      <c r="A60" s="60" t="s">
+        <v>151</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="70" t="s">
-        <v>151</v>
+      <c r="A61" s="60" t="s">
+        <v>148</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="70" t="s">
-        <v>149</v>
+      <c r="A62" s="60" t="s">
+        <v>146</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="70" t="s">
-        <v>145</v>
+      <c r="A63" s="60" t="s">
+        <v>142</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="70" t="s">
-        <v>143</v>
+      <c r="A64" s="60" t="s">
+        <v>140</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C67" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="7" t="s">
-        <v>120</v>
+      <c r="A71" s="55" t="s">
+        <v>494</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>119</v>
+        <v>493</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>118</v>
+        <v>495</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>117</v>
-      </c>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="B72" s="9"/>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="B73" s="9"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="B74" s="9"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="B75" s="9"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="65" t="s">
-        <v>493</v>
-      </c>
-      <c r="C76" s="7" t="s">
+      <c r="B76" s="9"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="55" t="s">
+        <v>487</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D81" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="66" t="s">
-        <v>494</v>
-      </c>
-      <c r="D77" s="8" t="s">
+    <row r="82" spans="1:4">
+      <c r="A82" s="56" t="s">
+        <v>488</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="57" t="s">
+        <v>489</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="58" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="60" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="7" t="s">
         <v>492</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="67" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="68" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="70" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="7" t="s">
-        <v>498</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="D76" r:id="rId2"/>
+    <hyperlink ref="D81" r:id="rId2"/>
     <hyperlink ref="B20" r:id="rId3"/>
     <hyperlink ref="B22" r:id="rId4"/>
     <hyperlink ref="B23" r:id="rId5"/>
@@ -3738,7 +3765,7 @@
     <hyperlink ref="B65" r:id="rId56"/>
     <hyperlink ref="B66" r:id="rId57"/>
     <hyperlink ref="B67" r:id="rId58"/>
-    <hyperlink ref="D77" r:id="rId59"/>
+    <hyperlink ref="D82" r:id="rId59"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId60"/>
@@ -3746,6 +3773,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="37.375" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
@@ -3799,617 +3845,617 @@
     <row r="2" spans="1:18" s="38" customFormat="1" ht="16.5" thickBot="1">
       <c r="A2" s="46"/>
       <c r="B2" s="45" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="45" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="H2" s="43"/>
       <c r="I2" s="44" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="J2" s="43"/>
       <c r="K2" s="45" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="M2" s="44" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="N2" s="43"/>
       <c r="O2" s="42" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="P2" s="41"/>
       <c r="Q2" s="40" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="R2" s="39"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="58" t="s">
-        <v>483</v>
+      <c r="A3" s="64" t="s">
+        <v>477</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="78.75">
-      <c r="A4" s="59"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="17" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="31.5">
-      <c r="A5" s="59"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="17" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E5" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>461</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>468</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>467</v>
-      </c>
       <c r="J5" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="31.5">
-      <c r="A6" s="59"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="17" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="31.5">
-      <c r="A7" s="59"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="17" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="59"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="17" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K8" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="O8" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>439</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>438</v>
-      </c>
       <c r="P8" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="59"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="17" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="59"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="17" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="L10" s="18"/>
       <c r="O10" s="14" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="20" customFormat="1">
-      <c r="A11" s="60"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="27" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="25"/>
       <c r="I11" s="26" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K11" s="27"/>
       <c r="M11" s="26"/>
       <c r="N11" s="25"/>
       <c r="O11" s="24" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q11" s="22" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="61" t="s">
-        <v>416</v>
+      <c r="A12" s="67" t="s">
+        <v>410</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="31.5">
-      <c r="A13" s="59"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="17" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="59"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="17" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="59"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="17" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="59"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="17" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="59"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="17" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="20" customFormat="1" ht="63">
-      <c r="A18" s="60"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="27" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="27" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="26" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="27" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="M18" s="26" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="N18" s="25"/>
       <c r="O18" s="24"/>
@@ -4418,407 +4464,407 @@
       <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="61" t="s">
-        <v>387</v>
+      <c r="A19" s="67" t="s">
+        <v>381</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="59"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="17" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="59"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="17" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I21" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q21" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="J21" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="L21" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="N21" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="O21" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="P21" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>367</v>
-      </c>
       <c r="R21" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="59"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="17" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="59"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="17" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="59"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="17" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="59"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D25" s="50" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J25" s="50" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="N25" s="50" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="48"/>
       <c r="R25" s="47"/>
     </row>
     <row r="26" spans="1:18" ht="16.5" thickBot="1">
-      <c r="A26" s="62"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="19" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="48"/>
@@ -4827,7 +4873,7 @@
     <row r="27" spans="1:18" s="38" customFormat="1" ht="16.5" thickBot="1">
       <c r="A27" s="46"/>
       <c r="B27" s="45" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C27" s="44" t="str">
         <f>C2</f>
@@ -4858,22 +4904,22 @@
       </c>
       <c r="N27" s="43"/>
       <c r="O27" s="42" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="P27" s="41"/>
       <c r="Q27" s="40"/>
       <c r="R27" s="39"/>
     </row>
     <row r="28" spans="1:18" s="18" customFormat="1">
-      <c r="A28" s="63" t="s">
-        <v>351</v>
+      <c r="A28" s="69" t="s">
+        <v>345</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E28" s="19"/>
       <c r="G28" s="16"/>
@@ -4889,13 +4935,13 @@
       <c r="R28" s="11"/>
     </row>
     <row r="29" spans="1:18" s="18" customFormat="1">
-      <c r="A29" s="56"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="37" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E29" s="19"/>
       <c r="G29" s="16"/>
@@ -4911,32 +4957,32 @@
       <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:18" s="18" customFormat="1">
-      <c r="A30" s="56"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="37" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="H30" s="15"/>
       <c r="I30" s="16" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="19" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="N30" s="15"/>
       <c r="O30" s="30"/>
@@ -4945,13 +4991,13 @@
       <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:18" s="18" customFormat="1">
-      <c r="A31" s="56"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="37" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E31" s="19"/>
       <c r="G31" s="16"/>
@@ -4967,12 +5013,12 @@
       <c r="R31" s="11"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="56"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="29" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K32" s="19"/>
       <c r="L32" s="18"/>
@@ -4980,12 +5026,12 @@
       <c r="P32" s="11"/>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="56"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="29" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K33" s="19"/>
       <c r="L33" s="18"/>
@@ -4993,12 +5039,12 @@
       <c r="P33" s="11"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="56"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="29" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="K34" s="19"/>
       <c r="L34" s="18"/>
@@ -5006,13 +5052,13 @@
       <c r="P34" s="11"/>
     </row>
     <row r="35" spans="1:18" s="20" customFormat="1">
-      <c r="A35" s="57"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="35" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="25" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="E35" s="34"/>
       <c r="G35" s="33"/>
@@ -5028,11 +5074,11 @@
       <c r="R35" s="21"/>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="55" t="s">
-        <v>335</v>
+      <c r="A36" s="61" t="s">
+        <v>329</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="K36" s="19"/>
       <c r="L36" s="18"/>
@@ -5040,9 +5086,9 @@
       <c r="P36" s="11"/>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="56"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="19" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="K37" s="19"/>
       <c r="L37" s="18"/>
@@ -5050,9 +5096,9 @@
       <c r="P37" s="11"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="56"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="19" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="K38" s="19"/>
       <c r="L38" s="18"/>
@@ -5060,9 +5106,9 @@
       <c r="P38" s="11"/>
     </row>
     <row r="39" spans="1:18" s="20" customFormat="1" ht="47.25">
-      <c r="A39" s="57"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="27" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="25"/>
@@ -5080,116 +5126,116 @@
       <c r="R39" s="21"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="55" t="s">
-        <v>330</v>
+      <c r="A40" s="61" t="s">
+        <v>324</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K40" s="19"/>
       <c r="L40" s="18"/>
       <c r="O40" s="30" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="P40" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="Q40" s="12" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="R40" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="31.5">
-      <c r="A41" s="56"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="29" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="K41" s="19"/>
       <c r="L41" s="18"/>
       <c r="O41" s="30" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="P41" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q41" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="Q41" s="12" t="s">
-        <v>325</v>
-      </c>
       <c r="R41" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="56"/>
+      <c r="A42" s="62"/>
       <c r="B42" s="29" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K42" s="19"/>
       <c r="L42" s="18"/>
       <c r="O42" s="30" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="P42" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="Q42" s="12" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="R42" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="56"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="29" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K43" s="19"/>
       <c r="L43" s="18"/>
       <c r="O43" s="30" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="P43" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="Q43" s="12" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="R43" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="56"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="29" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="20" customFormat="1">
-      <c r="A45" s="57"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="28" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="25" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E45" s="27"/>
       <c r="G45" s="26"/>
@@ -5219,7 +5265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D31"/>
   <sheetViews>
@@ -5235,10 +5281,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="20.25">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="64"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="4" spans="2:4" s="2" customFormat="1">
       <c r="B4" s="1">
@@ -5465,7 +5511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:F79"/>
   <sheetViews>
@@ -5481,10 +5527,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:6" ht="20.25">
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="64"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="4" spans="4:6">
       <c r="D4" s="4">
@@ -5798,7 +5844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E80"/>
   <sheetViews>
@@ -5814,10 +5860,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="20.25">
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="64"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="4" spans="3:5">
       <c r="C4" s="4">

</xml_diff>